<commit_message>
Made EXCEL FILE read-only
</commit_message>
<xml_diff>
--- a/templates/MS Excel/LogsTemplate.xlsx
+++ b/templates/MS Excel/LogsTemplate.xlsx
@@ -7,12 +7,10 @@
     <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Logs Sheet" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$3:$D$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Logs Sheet'!$A$3:$D$3</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
@@ -488,6 +486,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection password="D447" sheet="1" objects="1" scenarios="1"/>
   <autoFilter ref="A3:D3"/>
   <mergeCells count="2">
     <mergeCell ref="A1:D1"/>
@@ -496,28 +495,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>